<commit_message>
Code has been updated
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Checkout.xlsx
+++ b/src/test/java/com/born/xls/Checkout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -164,9 +164,6 @@
     <t>pause</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Select a product on plp page </t>
   </si>
   <si>
@@ -227,10 +224,13 @@
     <t>TS018</t>
   </si>
   <si>
-    <t>ProductDetails_Button</t>
-  </si>
-  <si>
     <t>TAILORED JUST TO YOU</t>
+  </si>
+  <si>
+    <t>ProductItem_Link</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -707,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -921,7 +921,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>47</v>
@@ -930,7 +930,7 @@
         <v>48</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -940,13 +940,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>70</v>
@@ -959,7 +959,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>47</v>
@@ -968,7 +968,7 @@
         <v>48</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -978,16 +978,16 @@
         <v>3</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -997,16 +997,16 @@
         <v>3</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>47</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -1016,16 +1016,16 @@
         <v>3</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -1035,16 +1035,16 @@
         <v>3</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
@@ -1054,16 +1054,16 @@
         <v>3</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -1073,7 +1073,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>23</v>
@@ -1091,11 +1091,11 @@
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -1207,7 +1207,7 @@
         <v>48</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -1220,10 +1220,10 @@
         <v>33</v>
       </c>
       <c r="C27" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>70</v>
@@ -1245,7 +1245,7 @@
         <v>48</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
@@ -1258,13 +1258,13 @@
         <v>35</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -1274,16 +1274,16 @@
         <v>4</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>47</v>
       </c>
       <c r="D30" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
@@ -1293,16 +1293,16 @@
         <v>4</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
@@ -1312,16 +1312,16 @@
         <v>4</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
@@ -1331,16 +1331,16 @@
         <v>4</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
@@ -1350,7 +1350,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>23</v>

</xml_diff>